<commit_message>
Lista de requisitos y seguimiento
</commit_message>
<xml_diff>
--- a/Documentos_proyecto/3.- Lista de requisitos y seguimiento_v1.xlsx
+++ b/Documentos_proyecto/3.- Lista de requisitos y seguimiento_v1.xlsx
@@ -432,28 +432,28 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="1" sqref="A1:M1 D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.0204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.0204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="66.3775510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="65.6071428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,7 +494,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
@@ -527,7 +527,7 @@
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
     </row>
-    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
@@ -589,7 +589,7 @@
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
     </row>
-    <row r="5" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="69.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
         <v>4</v>
       </c>
@@ -620,7 +620,7 @@
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
         <v>5</v>
       </c>
@@ -651,7 +651,7 @@
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="69.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
         <v>6</v>
       </c>
@@ -682,7 +682,7 @@
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
         <v>7</v>
       </c>
@@ -713,7 +713,7 @@
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
         <v>8</v>
       </c>
@@ -744,7 +744,7 @@
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
     </row>
-    <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
         <v>9</v>
       </c>
@@ -806,7 +806,7 @@
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
     </row>
-    <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="n">
         <v>11</v>
       </c>
@@ -837,7 +837,7 @@
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
     </row>
-    <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="n">
         <v>12</v>
       </c>
@@ -868,7 +868,7 @@
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
     </row>
-    <row r="14" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="24.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="n">
         <v>13</v>
       </c>
@@ -930,7 +930,7 @@
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
     </row>
-    <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="n">
         <v>15</v>
       </c>
@@ -961,7 +961,7 @@
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
     </row>
-    <row r="17" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="n">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Revisadas las diferencias de contenidos entre lo del repositorio y lo que tenian Victor y Patricio. Algunas correcciones de paso.
</commit_message>
<xml_diff>
--- a/Documentos_proyecto/3.- Lista de requisitos y seguimiento_v1.xlsx
+++ b/Documentos_proyecto/3.- Lista de requisitos y seguimiento_v1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="888" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="989"/>
+    <workbookView xWindow="1776" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -155,9 +155,6 @@
     <t>Si un turno se está regalando, sigue siendo del usuario inscrito con el hasta que otro usuario lo acepte.</t>
   </si>
   <si>
-    <t>MUY ALATA</t>
-  </si>
-  <si>
     <t>3.1</t>
   </si>
   <si>
@@ -243,6 +240,9 @@
   </si>
   <si>
     <t>No poder regalar todo los turnos.</t>
+  </si>
+  <si>
+    <t>MUY ALTA</t>
   </si>
 </sst>
 </file>
@@ -725,7 +725,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -787,7 +787,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -798,13 +798,13 @@
         <v>14</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>53</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="9" t="s">
@@ -817,7 +817,7 @@
         <v>18</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -839,7 +839,7 @@
         <v>15</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="9" t="s">
@@ -852,7 +852,7 @@
         <v>39</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -874,7 +874,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="9" t="s">
@@ -887,12 +887,12 @@
         <v>18</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -909,7 +909,7 @@
         <v>15</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="9" t="s">
@@ -922,12 +922,12 @@
         <v>16</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -944,7 +944,7 @@
         <v>15</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="9" t="s">
@@ -957,12 +957,12 @@
         <v>31</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -973,13 +973,13 @@
         <v>20</v>
       </c>
       <c r="D7" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="9" t="s">
@@ -992,12 +992,12 @@
         <v>31</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1008,13 +1008,13 @@
         <v>20</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="9" t="s">
@@ -1027,7 +1027,7 @@
         <v>31</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -1043,13 +1043,13 @@
         <v>20</v>
       </c>
       <c r="D9" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="9" t="s">
@@ -1059,15 +1059,15 @@
         <v>17</v>
       </c>
       <c r="J9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K9" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>44</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1078,13 +1078,13 @@
         <v>20</v>
       </c>
       <c r="D10" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>63</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="9" t="s">
@@ -1097,7 +1097,7 @@
         <v>16</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -1113,13 +1113,13 @@
         <v>20</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="9" t="s">
@@ -1132,7 +1132,7 @@
         <v>16</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -1148,7 +1148,7 @@
         <v>14</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>15</v>
@@ -1167,7 +1167,7 @@
         <v>31</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -1183,13 +1183,13 @@
         <v>20</v>
       </c>
       <c r="D13" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>67</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="9" t="s">
@@ -1202,7 +1202,7 @@
         <v>39</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -1218,7 +1218,7 @@
         <v>20</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>15</v>
@@ -1237,7 +1237,7 @@
         <v>39</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
@@ -1253,13 +1253,13 @@
         <v>20</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="9" t="s">
@@ -1272,12 +1272,12 @@
         <v>31</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -1288,13 +1288,13 @@
         <v>14</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="9" t="s">
@@ -1307,12 +1307,12 @@
         <v>16</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -1323,13 +1323,13 @@
         <v>20</v>
       </c>
       <c r="D17" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="9" t="s">
@@ -1342,7 +1342,7 @@
         <v>16</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>

</xml_diff>